<commit_message>
Implementado parcialmente HSBC, faltan HSBC, Santa
</commit_message>
<xml_diff>
--- a/bancomer.xlsx
+++ b/bancomer.xlsx
@@ -5,11 +5,11 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\proyectos\ScrapperCreditos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\proyectos\ScraperCreditos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="bancomer" sheetId="1" r:id="rId1"/>
@@ -941,7 +941,7 @@
   <dimension ref="A1:K285"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,7 +994,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3059,7 +3059,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3094,7 +3094,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3199,7 +3199,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3339,7 +3339,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3479,7 +3479,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3794,7 +3794,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3864,7 +3864,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3899,7 +3899,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3969,7 +3969,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4074,7 +4074,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4109,7 +4109,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -4179,7 +4179,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4249,7 +4249,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4389,7 +4389,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4459,7 +4459,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -4529,7 +4529,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -4564,7 +4564,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -4599,7 +4599,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -4634,7 +4634,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -4669,7 +4669,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -4704,7 +4704,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -4739,7 +4739,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -4809,7 +4809,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -4844,7 +4844,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -4879,7 +4879,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -4914,7 +4914,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4949,7 +4949,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4984,7 +4984,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -5019,7 +5019,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -5054,7 +5054,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -5089,7 +5089,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -5124,7 +5124,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -5194,7 +5194,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -5229,7 +5229,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -5264,7 +5264,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -5299,7 +5299,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -5334,7 +5334,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -5404,7 +5404,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -5439,7 +5439,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -5474,7 +5474,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -5509,7 +5509,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -5579,7 +5579,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -5614,7 +5614,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -5649,7 +5649,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -5684,7 +5684,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -5719,7 +5719,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -5754,7 +5754,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -5789,7 +5789,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -5824,7 +5824,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -5859,7 +5859,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -5894,7 +5894,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -5964,7 +5964,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
@@ -5999,7 +5999,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -6034,7 +6034,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -6069,7 +6069,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -6104,7 +6104,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -6139,7 +6139,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -6174,7 +6174,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
@@ -6209,7 +6209,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
@@ -6244,7 +6244,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
@@ -6279,7 +6279,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
@@ -6349,7 +6349,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
@@ -6384,7 +6384,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
@@ -6419,7 +6419,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
@@ -6454,7 +6454,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -6489,7 +6489,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
@@ -6524,7 +6524,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
@@ -6559,7 +6559,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
@@ -6594,7 +6594,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
@@ -6629,7 +6629,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
@@ -6664,7 +6664,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
@@ -6734,7 +6734,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>165</v>
       </c>
@@ -6769,7 +6769,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
@@ -6804,7 +6804,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>167</v>
       </c>
@@ -6839,7 +6839,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
@@ -6874,7 +6874,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>
@@ -6909,7 +6909,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>170</v>
       </c>
@@ -6944,7 +6944,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>171</v>
       </c>
@@ -6979,7 +6979,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>172</v>
       </c>
@@ -7014,7 +7014,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>173</v>
       </c>
@@ -7049,7 +7049,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>174</v>
       </c>
@@ -7119,7 +7119,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
@@ -7154,7 +7154,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>177</v>
       </c>
@@ -7189,7 +7189,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>178</v>
       </c>
@@ -7224,7 +7224,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>179</v>
       </c>
@@ -7259,7 +7259,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>180</v>
       </c>
@@ -7294,7 +7294,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>181</v>
       </c>
@@ -7364,7 +7364,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>183</v>
       </c>
@@ -7399,7 +7399,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>184</v>
       </c>
@@ -7434,7 +7434,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>185</v>
       </c>
@@ -7504,7 +7504,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>187</v>
       </c>
@@ -7539,7 +7539,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>188</v>
       </c>
@@ -7574,7 +7574,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>189</v>
       </c>
@@ -7609,7 +7609,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>190</v>
       </c>
@@ -7644,7 +7644,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>191</v>
       </c>
@@ -7679,7 +7679,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>192</v>
       </c>
@@ -7714,7 +7714,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>193</v>
       </c>
@@ -7749,7 +7749,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>194</v>
       </c>
@@ -7784,7 +7784,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>195</v>
       </c>
@@ -7819,7 +7819,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>196</v>
       </c>
@@ -7889,7 +7889,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>198</v>
       </c>
@@ -7924,7 +7924,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>199</v>
       </c>
@@ -7959,7 +7959,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>200</v>
       </c>
@@ -7994,7 +7994,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>201</v>
       </c>
@@ -8029,7 +8029,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>202</v>
       </c>
@@ -8064,7 +8064,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>203</v>
       </c>
@@ -8099,7 +8099,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>204</v>
       </c>
@@ -8134,7 +8134,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>205</v>
       </c>
@@ -8169,7 +8169,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>206</v>
       </c>
@@ -8204,7 +8204,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>207</v>
       </c>
@@ -8274,7 +8274,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>209</v>
       </c>
@@ -8309,7 +8309,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>210</v>
       </c>
@@ -8344,7 +8344,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>211</v>
       </c>
@@ -8379,7 +8379,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>212</v>
       </c>
@@ -8414,7 +8414,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>213</v>
       </c>
@@ -8449,7 +8449,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>214</v>
       </c>
@@ -8484,7 +8484,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>215</v>
       </c>
@@ -8519,7 +8519,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>216</v>
       </c>
@@ -8659,7 +8659,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>220</v>
       </c>
@@ -8694,7 +8694,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>221</v>
       </c>
@@ -8729,7 +8729,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>222</v>
       </c>
@@ -8764,7 +8764,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>223</v>
       </c>
@@ -8799,7 +8799,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>224</v>
       </c>
@@ -8834,7 +8834,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>225</v>
       </c>
@@ -8869,7 +8869,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>226</v>
       </c>
@@ -8904,7 +8904,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>227</v>
       </c>
@@ -8939,7 +8939,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>228</v>
       </c>
@@ -8974,7 +8974,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>229</v>
       </c>
@@ -9044,7 +9044,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>231</v>
       </c>
@@ -9079,7 +9079,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>232</v>
       </c>
@@ -9114,7 +9114,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>233</v>
       </c>
@@ -9149,7 +9149,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>234</v>
       </c>
@@ -9184,7 +9184,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>235</v>
       </c>
@@ -9219,7 +9219,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>236</v>
       </c>
@@ -9254,7 +9254,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>237</v>
       </c>
@@ -9289,7 +9289,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>238</v>
       </c>
@@ -9324,7 +9324,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>239</v>
       </c>
@@ -9359,7 +9359,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>240</v>
       </c>
@@ -9429,7 +9429,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>242</v>
       </c>
@@ -9464,7 +9464,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>243</v>
       </c>
@@ -9499,7 +9499,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>244</v>
       </c>
@@ -9534,7 +9534,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>245</v>
       </c>
@@ -9569,7 +9569,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>246</v>
       </c>
@@ -9604,7 +9604,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>247</v>
       </c>
@@ -9639,7 +9639,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>248</v>
       </c>
@@ -9674,7 +9674,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>249</v>
       </c>
@@ -9709,7 +9709,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>250</v>
       </c>
@@ -9744,7 +9744,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>251</v>
       </c>
@@ -9814,7 +9814,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>253</v>
       </c>
@@ -9849,7 +9849,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>254</v>
       </c>
@@ -9884,7 +9884,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>255</v>
       </c>
@@ -9919,7 +9919,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>256</v>
       </c>
@@ -9954,7 +9954,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>257</v>
       </c>
@@ -9989,7 +9989,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>258</v>
       </c>
@@ -10024,7 +10024,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>259</v>
       </c>
@@ -10059,7 +10059,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>260</v>
       </c>
@@ -10094,7 +10094,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>261</v>
       </c>
@@ -10129,7 +10129,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>262</v>
       </c>
@@ -10199,7 +10199,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>264</v>
       </c>
@@ -10234,7 +10234,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>265</v>
       </c>
@@ -10269,7 +10269,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>266</v>
       </c>
@@ -10304,7 +10304,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>267</v>
       </c>
@@ -10339,7 +10339,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>268</v>
       </c>
@@ -10374,7 +10374,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>269</v>
       </c>
@@ -10409,7 +10409,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>270</v>
       </c>
@@ -10444,7 +10444,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>271</v>
       </c>
@@ -10479,7 +10479,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>272</v>
       </c>
@@ -10514,7 +10514,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>273</v>
       </c>
@@ -10584,7 +10584,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>275</v>
       </c>
@@ -10619,7 +10619,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>276</v>
       </c>
@@ -10654,7 +10654,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>277</v>
       </c>
@@ -10689,7 +10689,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>278</v>
       </c>
@@ -10724,7 +10724,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>279</v>
       </c>
@@ -10759,7 +10759,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>280</v>
       </c>
@@ -10794,7 +10794,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>281</v>
       </c>
@@ -10829,7 +10829,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>282</v>
       </c>
@@ -10864,7 +10864,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>283</v>
       </c>
@@ -10899,7 +10899,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>284</v>
       </c>
@@ -10936,148 +10936,13 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K285">
-    <filterColumn colId="8">
+    <filterColumn colId="3">
       <filters>
-        <filter val="101.50%"/>
-        <filter val="107.30%"/>
-        <filter val="114.20%"/>
-        <filter val="119.40%"/>
-        <filter val="145.40%"/>
-        <filter val="145.60%"/>
-        <filter val="145.70%"/>
-        <filter val="145.80%"/>
-        <filter val="147.50%"/>
-        <filter val="147.70%"/>
-        <filter val="148.40%"/>
-        <filter val="149.50%"/>
-        <filter val="152.40%"/>
-        <filter val="155.00%"/>
-        <filter val="160.20%"/>
-        <filter val="161.90%"/>
-        <filter val="165.30%"/>
-        <filter val="166.80%"/>
-        <filter val="171.30%"/>
-        <filter val="171.70%"/>
-        <filter val="174.00%"/>
-        <filter val="183.20%"/>
-        <filter val="244.70%"/>
-        <filter val="245.60%"/>
-        <filter val="248.40%"/>
-        <filter val="254.50%"/>
-        <filter val="257.70%"/>
-        <filter val="260.40%"/>
-        <filter val="263.60%"/>
-        <filter val="264.70%"/>
-        <filter val="267.10%"/>
-        <filter val="268.50%"/>
-        <filter val="269.20%"/>
-        <filter val="270.90%"/>
-        <filter val="279.00%"/>
-        <filter val="286.00%"/>
-        <filter val="288.80%"/>
-        <filter val="291.40%"/>
-        <filter val="295.20%"/>
-        <filter val="297.90%"/>
-        <filter val="30.90%"/>
-        <filter val="31.10%"/>
-        <filter val="31.40%"/>
-        <filter val="31.70%"/>
-        <filter val="310.70%"/>
-        <filter val="313.40%"/>
-        <filter val="314.20%"/>
-        <filter val="317.10%"/>
-        <filter val="32.00%"/>
-        <filter val="32.40%"/>
-        <filter val="32.80%"/>
-        <filter val="322.50%"/>
-        <filter val="33.30%"/>
-        <filter val="33.80%"/>
-        <filter val="34.50%"/>
-        <filter val="349.60%"/>
-        <filter val="35.20%"/>
-        <filter val="36.10%"/>
-        <filter val="37.20%"/>
-        <filter val="38.40%"/>
-        <filter val="381.10%"/>
-        <filter val="383.80%"/>
-        <filter val="40.10%"/>
-        <filter val="41.60%"/>
-        <filter val="415.60%"/>
-        <filter val="424.20%"/>
-        <filter val="461.10%"/>
-        <filter val="519.20%"/>
-        <filter val="52.20%"/>
-        <filter val="52.30%"/>
-        <filter val="52.80%"/>
-        <filter val="52.90%"/>
-        <filter val="523.10%"/>
-        <filter val="53.40%"/>
-        <filter val="53.60%"/>
-        <filter val="53.70%"/>
-        <filter val="535.30%"/>
-        <filter val="538.30%"/>
-        <filter val="539.90%"/>
-        <filter val="54.40%"/>
-        <filter val="54.50%"/>
-        <filter val="549.90%"/>
-        <filter val="55.30%"/>
-        <filter val="551.20%"/>
-        <filter val="56.40%"/>
-        <filter val="563.00%"/>
-        <filter val="566.00%"/>
-        <filter val="57.80%"/>
-        <filter val="579.30%"/>
-        <filter val="59.40%"/>
-        <filter val="592.40%"/>
-        <filter val="596.10%"/>
-        <filter val="601.10%"/>
-        <filter val="61.40%"/>
-        <filter val="610.40%"/>
-        <filter val="619.20%"/>
-        <filter val="625.80%"/>
-        <filter val="631.30%"/>
-        <filter val="637.20%"/>
-        <filter val="64.00%"/>
-        <filter val="645.00%"/>
-        <filter val="661.00%"/>
-        <filter val="666.50%"/>
-        <filter val="67.20%"/>
-        <filter val="680.70%"/>
-        <filter val="682.90%"/>
-        <filter val="70.90%"/>
-        <filter val="701.00%"/>
-        <filter val="703.40%"/>
-        <filter val="719.90%"/>
-        <filter val="73.70%"/>
-        <filter val="741.20%"/>
-        <filter val="744.70%"/>
-        <filter val="765.20%"/>
-        <filter val="798.40%"/>
-        <filter val="806.40%"/>
-        <filter val="834.60%"/>
-        <filter val="839.80%"/>
-        <filter val="85.60%"/>
-        <filter val="86.30%"/>
-        <filter val="87.00%"/>
-        <filter val="87.20%"/>
-        <filter val="87.70%"/>
-        <filter val="88.70%"/>
-        <filter val="89.70%"/>
-        <filter val="89.90%"/>
-        <filter val="90.50%"/>
-        <filter val="91.40%"/>
-        <filter val="910.00%"/>
-        <filter val="914.50%"/>
-        <filter val="930.60%"/>
-        <filter val="933.20%"/>
-        <filter val="94.00%"/>
-        <filter val="95.90%"/>
-        <filter val="960.90%"/>
-        <filter val="97.30%"/>
-        <filter val="97.70%"/>
-        <filter val="971.90%"/>
-        <filter val="976.30%"/>
-        <filter val="995.40%"/>
+        <filter val="40.00%"/>
+        <filter val="70.00%"/>
+        <filter val="76.58%"/>
+        <filter val="85.00%"/>
+        <filter val="90.00%"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>